<commit_message>
thms results and data added
</commit_message>
<xml_diff>
--- a/equivalence_clust_data/DescriptorAnnotations_Edgar.xlsx
+++ b/equivalence_clust_data/DescriptorAnnotations_Edgar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmadapan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AHRQ\AHRQ-Gesture-Videos\Agreement-Analysis\equivalence_clust_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -495,9 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -538,12 +536,8 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -561,9 +555,7 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -581,9 +573,7 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -686,9 +676,7 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -706,9 +694,7 @@
       <c r="E11" s="1">
         <v>1</v>
       </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -726,12 +712,8 @@
       <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -749,12 +731,8 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -772,9 +750,7 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -792,12 +768,8 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -815,12 +787,8 @@
       <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -838,12 +806,8 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -861,15 +825,9 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
-        <v>1</v>
-      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -887,9 +845,7 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -907,15 +863,9 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1</v>
-      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -933,21 +883,11 @@
       <c r="E21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4">
-        <v>1</v>
-      </c>
-      <c r="I21" s="4">
-        <v>1</v>
-      </c>
-      <c r="J21" s="4">
-        <v>1</v>
-      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -965,21 +905,11 @@
       <c r="E22" s="1">
         <v>1</v>
       </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1</v>
-      </c>
-      <c r="J22" s="4">
-        <v>1</v>
-      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -997,21 +927,11 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1</v>
-      </c>
-      <c r="J23" s="4">
-        <v>1</v>
-      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1029,15 +949,9 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4">
-        <v>1</v>
-      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -1055,21 +969,11 @@
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1</v>
-      </c>
-      <c r="H25" s="4">
-        <v>1</v>
-      </c>
-      <c r="I25" s="4">
-        <v>1</v>
-      </c>
-      <c r="J25" s="4">
-        <v>1</v>
-      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -1087,18 +991,10 @@
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4">
-        <v>1</v>
-      </c>
-      <c r="I26" s="4">
-        <v>1</v>
-      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1116,21 +1012,11 @@
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="3">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1</v>
-      </c>
-      <c r="J27" s="4">
-        <v>1</v>
-      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1148,24 +1034,12 @@
       <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1">
-        <v>1</v>
-      </c>
-      <c r="J28" s="1">
-        <v>1</v>
-      </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1183,21 +1057,11 @@
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="4">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1</v>
-      </c>
-      <c r="J29" s="4">
-        <v>1</v>
-      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>